<commit_message>
Migrated to gradle version, removed wrong inputType in xml, changed subpackage into lower case notation
</commit_message>
<xml_diff>
--- a/documentation/PouleAppDocumentation.xlsx
+++ b/documentation/PouleAppDocumentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="9" r:id="rId1"/>
@@ -472,7 +472,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,8 +515,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -570,12 +576,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -599,7 +671,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1404,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1536,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G39"/>
+  <dimension ref="B1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,301 +1631,313 @@
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="C2" s="24"/>
+      <c r="F2" s="29" t="s">
         <v>77</v>
       </c>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="26" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="3" t="s">
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="23" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="18" t="s">
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="C9" s="24"/>
+      <c r="F9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="25" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="25" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="25" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="25" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="18" t="s">
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="C16" s="24"/>
+      <c r="F16" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="22" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="s">
         <v>69</v>
       </c>
+      <c r="C21" s="24"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="18" t="s">
+    <row r="24" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+    <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="s">
         <v>90</v>
       </c>
+      <c r="C27" s="24"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
         <v>95</v>
       </c>
+      <c r="C33" s="24"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="B34" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="B35" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="20" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="B36" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="B37" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B38" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="39" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="22" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3821,11 +3915,11 @@
         <v>0</v>
       </c>
       <c r="AA44" s="7">
-        <f t="shared" ref="AA44:AA75" si="9">MOD($Z$10-Z44-Y44, $Z$10)</f>
+        <f t="shared" ref="AA44:AA67" si="9">MOD($Z$10-Z44-Y44, $Z$10)</f>
         <v>3</v>
       </c>
       <c r="AB44" s="7">
-        <f t="shared" ref="AB44:AB75" si="10">IF(AA44=Y44,MOD(Y44+($Z$10/2),$Z$10),AA44)</f>
+        <f t="shared" ref="AB44:AB67" si="10">IF(AA44=Y44,MOD(Y44+($Z$10/2),$Z$10),AA44)</f>
         <v>3</v>
       </c>
       <c r="AC44" s="7" t="b">

</xml_diff>